<commit_message>
minor fixes + qkv method
</commit_message>
<xml_diff>
--- a/notebooks/metrics.xlsx
+++ b/notebooks/metrics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\60130060\aibek_diploma\notebooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9D64C4C9-4667-4348-BF18-C624D86ED7E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7574EA2B-FCFB-41F7-A804-6CF90B86505B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="58">
   <si>
     <t>CLIP-I</t>
   </si>
@@ -55,9 +54,6 @@
     <t>Custom Diffusion</t>
   </si>
   <si>
-    <t>0.89239824</t>
-  </si>
-  <si>
     <t>SVDiff</t>
   </si>
   <si>
@@ -67,145 +63,170 @@
     <t>cat</t>
   </si>
   <si>
-    <t>0.81522125</t>
-  </si>
-  <si>
     <t>G-R</t>
   </si>
   <si>
-    <t>0.93100274</t>
-  </si>
-  <si>
-    <t>0.8773863</t>
-  </si>
-  <si>
-    <t>0.24834694</t>
-  </si>
-  <si>
-    <t>0.24252953</t>
-  </si>
-  <si>
-    <t>0.8576475</t>
-  </si>
-  <si>
-    <t>0.25906914</t>
-  </si>
-  <si>
-    <t>0.8447423</t>
-  </si>
-  <si>
-    <t>0.24493115</t>
-  </si>
-  <si>
-    <t>0.8489554</t>
-  </si>
-  <si>
-    <t>0.86719936</t>
-  </si>
-  <si>
-    <t>0.23255336</t>
-  </si>
-  <si>
-    <t>0.84281194</t>
-  </si>
-  <si>
-    <t>0.82979965</t>
-  </si>
-  <si>
-    <t>0.24143207</t>
-  </si>
-  <si>
-    <t>0.7998256</t>
-  </si>
-  <si>
-    <t>0.8319386</t>
-  </si>
-  <si>
-    <t>0.25059816</t>
-  </si>
-  <si>
-    <t>0.9156026</t>
-  </si>
-  <si>
-    <t>0.85692525</t>
-  </si>
-  <si>
-    <t>0.23155773</t>
-  </si>
-  <si>
-    <t>0.87776536</t>
-  </si>
-  <si>
-    <t>0.25758153</t>
-  </si>
-  <si>
-    <t>0.8722472</t>
-  </si>
-  <si>
-    <t>0.8353296</t>
-  </si>
-  <si>
-    <t>0.2611505</t>
-  </si>
-  <si>
-    <t>0.88762975</t>
-  </si>
-  <si>
-    <t>0.8313288</t>
-  </si>
-  <si>
-    <t>0.24082369</t>
-  </si>
-  <si>
-    <t>0.8352455</t>
-  </si>
-  <si>
-    <t>0.79722285</t>
-  </si>
-  <si>
-    <t>0.24151613</t>
-  </si>
-  <si>
-    <t>0.89735985</t>
-  </si>
-  <si>
-    <t>0.8452155</t>
-  </si>
-  <si>
-    <t>0.20244536</t>
-  </si>
-  <si>
-    <t>0.8549101</t>
-  </si>
-  <si>
-    <t>0.82322073</t>
-  </si>
-  <si>
-    <t>0.21698892</t>
-  </si>
-  <si>
-    <t>0.8159798</t>
-  </si>
-  <si>
-    <t>0.7837137</t>
-  </si>
-  <si>
-    <t>0.22100945</t>
-  </si>
-  <si>
-    <t>0.8858522</t>
+    <t>0.2617249</t>
+  </si>
+  <si>
+    <t>0.93363905</t>
+  </si>
+  <si>
+    <t>0.8500741</t>
+  </si>
+  <si>
+    <t>0.23833336</t>
+  </si>
+  <si>
+    <t>0.8685597</t>
+  </si>
+  <si>
+    <t>0.8602076</t>
+  </si>
+  <si>
+    <t>0.23220457</t>
+  </si>
+  <si>
+    <t>0.93991476</t>
+  </si>
+  <si>
+    <t>0.9086448</t>
+  </si>
+  <si>
+    <t>0.25089368</t>
+  </si>
+  <si>
+    <t>0.87964493</t>
+  </si>
+  <si>
+    <t>0.82912034</t>
+  </si>
+  <si>
+    <t>0.23843332</t>
+  </si>
+  <si>
+    <t>0.81603616</t>
+  </si>
+  <si>
+    <t>0.81025904</t>
+  </si>
+  <si>
+    <t>0.25188205</t>
+  </si>
+  <si>
+    <t>0.88389564</t>
+  </si>
+  <si>
+    <t>0.83535695</t>
+  </si>
+  <si>
+    <t>0.26388216</t>
+  </si>
+  <si>
+    <t>0.90636194</t>
+  </si>
+  <si>
+    <t>0.84326714</t>
+  </si>
+  <si>
+    <t>0.23933922</t>
+  </si>
+  <si>
+    <t>0.8913542</t>
+  </si>
+  <si>
+    <t>0.8639414</t>
+  </si>
+  <si>
+    <t>0.25468722</t>
+  </si>
+  <si>
+    <t>0.91548</t>
+  </si>
+  <si>
+    <t>0.8735388</t>
+  </si>
+  <si>
+    <t>0.25381148</t>
+  </si>
+  <si>
+    <t>0.93874496</t>
+  </si>
+  <si>
+    <t>0.87340903</t>
+  </si>
+  <si>
+    <t>0.9107676</t>
+  </si>
+  <si>
+    <t>0.84909487</t>
+  </si>
+  <si>
+    <t>0.25568956</t>
+  </si>
+  <si>
+    <t>0.9261573</t>
+  </si>
+  <si>
+    <t>0.86479485</t>
+  </si>
+  <si>
+    <t>0.24985662</t>
+  </si>
+  <si>
+    <t>0.9360693</t>
+  </si>
+  <si>
+    <t>0.8702746</t>
+  </si>
+  <si>
+    <t>0.23673433</t>
+  </si>
+  <si>
+    <t>0.889</t>
+  </si>
+  <si>
+    <t>0.8554526</t>
+  </si>
+  <si>
+    <t>0.23737207</t>
+  </si>
+  <si>
+    <t>0.9375689</t>
+  </si>
+  <si>
+    <t>0.8985749</t>
+  </si>
+  <si>
+    <t>0.24197556</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -237,12 +258,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -526,7 +549,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -551,7 +574,7 @@
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -562,13 +585,13 @@
         <v>4</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>49</v>
+        <v>23</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>48</v>
+        <v>22</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>50</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -579,13 +602,13 @@
         <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -596,13 +619,13 @@
         <v>4</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>15</v>
+        <v>49</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>17</v>
+        <v>48</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>16</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -619,24 +642,24 @@
         <v>31</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>9</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>39</v>
-      </c>
       <c r="E6" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -644,16 +667,16 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>52</v>
+        <v>26</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>51</v>
+        <v>25</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>53</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -661,16 +684,16 @@
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -678,16 +701,16 @@
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>19</v>
+        <v>52</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>18</v>
+        <v>51</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>19</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -695,30 +718,30 @@
         <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>35</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>34</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>11</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>42</v>
+      <c r="D11" s="4" t="s">
+        <v>57</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>44</v>
@@ -729,16 +752,16 @@
         <v>5</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>55</v>
+        <v>29</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>54</v>
+        <v>28</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -746,16 +769,16 @@
         <v>6</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -763,16 +786,16 @@
         <v>7</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>21</v>
+        <v>55</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>20</v>
+        <v>54</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
@@ -780,24 +803,24 @@
         <v>8</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C15" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D15" s="2" t="s">
-        <v>36</v>
-      </c>
       <c r="E15" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>46</v>

</xml_diff>